<commit_message>
Added Boundaries. Made the app use much less memory.
</commit_message>
<xml_diff>
--- a/App/CollisionMasks.xlsx
+++ b/App/CollisionMasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13220" yWindow="40" windowWidth="12760" windowHeight="15560" tabRatio="500"/>
+    <workbookView xWindow="12760" yWindow="0" windowWidth="12760" windowHeight="15560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
   <si>
     <t>Player Bullets</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Enemy Ship</t>
   </si>
   <si>
-    <t>Enemy Bullets</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -43,6 +40,15 @@
   </si>
   <si>
     <t>SUM</t>
+  </si>
+  <si>
+    <t>Enemy Bullets Limited</t>
+  </si>
+  <si>
+    <t>Enemy Bullets No Boundaries</t>
+  </si>
+  <si>
+    <t>Boundaries</t>
   </si>
 </sst>
 </file>
@@ -98,8 +104,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -113,15 +123,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -451,19 +465,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="2.83203125" customWidth="1"/>
+    <col min="4" max="4" width="4.1640625" customWidth="1"/>
+    <col min="5" max="5" width="2.6640625" customWidth="1"/>
+    <col min="6" max="6" width="3" customWidth="1"/>
+    <col min="7" max="7" width="3.1640625" customWidth="1"/>
+    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="9" max="9" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="C1">
         <v>1</v>
       </c>
@@ -476,114 +497,179 @@
       <c r="F1">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="G1">
+        <v>16</v>
+      </c>
+      <c r="H1">
+        <v>32</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="I2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>5</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="I7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
       <c r="F8" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="I8">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="I9">
         <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>